<commit_message>
Modifying the generating documents.
</commit_message>
<xml_diff>
--- a/data/form1.xlsx
+++ b/data/form1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dflores/Dropbox/EXTS/Projects/autoHiring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45F32F0-3D03-6646-9F03-915C4F36E435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D389A600-3412-674B-A36B-9A097A8C3461}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="24820" windowHeight="28340" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
+    <workbookView xWindow="26380" yWindow="14640" windowWidth="24820" windowHeight="14180" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="108">
   <si>
     <t>First Name</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>Data Science Course Developer and Instructor - R</t>
-  </si>
-  <si>
-    <t>756.6576.5019.29</t>
   </si>
   <si>
     <t>Geneva</t>
@@ -439,7 +436,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -473,11 +470,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -562,6 +570,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -880,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D2E135-155D-3F42-BE22-6B196658E3B7}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,10 +919,10 @@
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>89</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>33</v>
@@ -929,7 +940,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -941,22 +952,20 @@
         <v>32</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>82</v>
-      </c>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
@@ -979,7 +988,7 @@
         <v>68</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -999,7 +1008,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1035,15 +1044,15 @@
         <v>71</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15" s="24">
         <v>2</v>
@@ -1052,16 +1061,16 @@
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="24" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1078,13 +1087,13 @@
     </row>
     <row r="18" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>63</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="23"/>
     </row>
@@ -1109,7 +1118,7 @@
         <v>74</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1126,10 +1135,10 @@
     </row>
     <row r="22" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>76</v>
@@ -1140,7 +1149,7 @@
     </row>
     <row r="23" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>61</v>
@@ -1148,11 +1157,11 @@
       <c r="C23" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="23"/>
-    </row>
-    <row r="24" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="D23" s="34"/>
+    </row>
+    <row r="24" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>67</v>
@@ -1164,10 +1173,10 @@
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>98</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>99</v>
       </c>
       <c r="C25" s="25">
         <v>44105</v>
@@ -1194,7 +1203,7 @@
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>80</v>
@@ -1202,7 +1211,7 @@
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="28"/>
       <c r="C28" s="29">
@@ -1217,13 +1226,13 @@
         <v>58</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1505,9 +1514,9 @@
       <c r="A12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="8" t="str">
+      <c r="B12" s="8">
         <f>Details!D7</f>
-        <v>756.6576.5019.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>